<commit_message>
Se actualiza cronograma a versión 2
Se actualiza cronograma a versión 2
</commit_message>
<xml_diff>
--- a/Documentos/Cronograma de Actividades_V.1.1.2.xlsx
+++ b/Documentos/Cronograma de Actividades_V.1.1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erika\Documents\GitHub\Documentation\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{820C39F9-1011-4657-BCC4-5BCC5D88A8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34FCE82-ED67-46AF-96DD-A24E5827DAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B9DA602-071F-4FD7-9752-666F02B18691}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_Hlk210645862" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3675,7 +3674,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>